<commit_message>
máquinas de estado feita
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita.xlsx
+++ b/use-cases/use-case-realizar-receita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/projeto-li4/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43FF808-366A-1447-970D-B22339F42B93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A365DD1-A4E6-264B-903D-8AB5F6A41B86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>4.1. o passo anterior é apresentado no ecrã.</t>
   </si>
   <si>
-    <t>4.2.  regressa ao passo 3.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Alternativa 2
 [ator </t>
@@ -129,11 +126,6 @@
     </r>
   </si>
   <si>
-    <t>Alternativa 3
-[ator carrega no botão "Finish"]
-(passo 4)</t>
-  </si>
-  <si>
     <t>4.1. &lt;&lt;include&gt;&gt; quiz</t>
   </si>
   <si>
@@ -155,6 +147,15 @@
   </si>
   <si>
     <t>Cliente</t>
+  </si>
+  <si>
+    <t>Alternativa 3
+[ator encontra-se no último passo
+ e carrega no botão "Finish"]
+(passo 4)</t>
+  </si>
+  <si>
+    <t>4.2.  regressa a 3.</t>
   </si>
 </sst>
 </file>
@@ -747,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -774,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="18"/>
     </row>
@@ -798,7 +799,7 @@
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
       <c r="B6" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -848,12 +849,12 @@
       <c r="B12" s="16"/>
       <c r="C12" s="7"/>
       <c r="D12" s="9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="46" customHeight="1" thickBot="1">
       <c r="B13" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="13" t="s">
@@ -864,39 +865,39 @@
       <c r="B14" s="16"/>
       <c r="C14" s="7"/>
       <c r="D14" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="40" customHeight="1" thickBot="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="47" customHeight="1" thickBot="1">
       <c r="B15" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="32" customHeight="1" thickBot="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="43" customHeight="1" thickBot="1">
       <c r="B16" s="16"/>
       <c r="C16" s="7"/>
       <c r="D16" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="43" customHeight="1" thickBot="1">
       <c r="B17" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="44" customHeight="1" thickBot="1">
       <c r="B18" s="16"/>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use case realizar receita feito
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita.xlsx
+++ b/use-cases/use-case-realizar-receita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/projeto-li4/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A365DD1-A4E6-264B-903D-8AB5F6A41B86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B96A3B8-9F7E-1B4E-BBF8-EEAB122497A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Actor input</t>
   </si>
@@ -63,7 +63,12 @@
     <t>3. Ator carrega num botão.</t>
   </si>
   <si>
-    <t>4. sistema interpreta botão carregado.</t>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Cenário 
+Normal</t>
   </si>
   <si>
     <r>
@@ -89,14 +94,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> se encontra no último passo e carrega no botão "Avançar"]
-(passo 4)</t>
+(passo 3)</t>
     </r>
-  </si>
-  <si>
-    <t>4.1. o passo seguinte é apresentado no ecrã.</t>
-  </si>
-  <si>
-    <t>4.1. o passo anterior é apresentado no ecrã.</t>
   </si>
   <si>
     <r>
@@ -122,40 +121,41 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> se encontra no passo 1 e carrega no botão "Recuar"]
-(passo 4)</t>
+(passo 3)</t>
     </r>
   </si>
   <si>
-    <t>4.1. &lt;&lt;include&gt;&gt; quiz</t>
-  </si>
-  <si>
-    <t>4.2. regressa ao menu principal.</t>
+    <t>Alternativa 3
+[ator encontra-se no último passo
+ e carrega no botão "Finish"]
+(passo 3)</t>
   </si>
   <si>
     <t>Alternativa 4
 [ator carrega no botão numa 
 expressão para pesquisa]
-(passo 4)</t>
-  </si>
-  <si>
-    <t>4.1. &lt;&lt;include&gt;&gt; pesquisa expressão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Cenário 
-Normal</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Alternativa 3
-[ator encontra-se no último passo
- e carrega no botão "Finish"]
-(passo 4)</t>
-  </si>
-  <si>
-    <t>4.2.  regressa a 3.</t>
+(passo 3)</t>
+  </si>
+  <si>
+    <t>3.1. &lt;&lt;include&gt;&gt; pesquisa expressão</t>
+  </si>
+  <si>
+    <t>3.2. regressa ao menu principal.</t>
+  </si>
+  <si>
+    <t>3.1. &lt;&lt;include&gt;&gt; quiz</t>
+  </si>
+  <si>
+    <t>3.1. o passo anterior é apresentado no ecrã.</t>
+  </si>
+  <si>
+    <t>3.1. o passo seguinte é apresentado no ecrã.</t>
+  </si>
+  <si>
+    <t>3.2.  o processo é encerrado.</t>
+  </si>
+  <si>
+    <t>3.2. o processo é encerrado.</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -357,24 +357,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -404,9 +391,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -746,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D18"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -765,41 +749,41 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="18"/>
+      <c r="C3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="21" t="s">
-        <v>21</v>
+      <c r="B6" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -809,108 +793,101 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1">
-      <c r="B7" s="21"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1">
-      <c r="B9" s="22"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="2:4" ht="25" customHeight="1" thickBot="1">
-      <c r="B10" s="22"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" s="12" customFormat="1" ht="43" customHeight="1" thickBot="1">
-      <c r="B11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="13" t="s">
+    <row r="10" spans="2:4" s="12" customFormat="1" ht="43" customHeight="1" thickBot="1">
+      <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="46" customHeight="1" thickBot="1">
+      <c r="B11" s="15"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:4" ht="46" customHeight="1" thickBot="1">
-      <c r="B12" s="16"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="41" customHeight="1" thickBot="1">
+      <c r="B13" s="15"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="46" customHeight="1" thickBot="1">
-      <c r="B13" s="15" t="s">
+    <row r="14" spans="2:4" ht="47" customHeight="1" thickBot="1">
+      <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="41" customHeight="1" thickBot="1">
-      <c r="B14" s="16"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="47" customHeight="1" thickBot="1">
-      <c r="B15" s="15" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="43" customHeight="1" thickBot="1">
+      <c r="B15" s="15"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="43" customHeight="1" thickBot="1">
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="44" customHeight="1" thickBot="1">
+      <c r="B17" s="15"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="43" customHeight="1" thickBot="1">
-      <c r="B16" s="16"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="43" customHeight="1" thickBot="1">
-      <c r="B17" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="44" customHeight="1" thickBot="1">
-      <c r="B18" s="16"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>